<commit_message>
[feat]: + Cancel booking API + add background service for flight and booking + add view total and remain seat
</commit_message>
<xml_diff>
--- a/flight_ticket_class_data.xlsx
+++ b/flight_ticket_class_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FBT\Kì 8\PRN231\PRN231Fall2024_SE1714_Group5_ARS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRN231\GroupProject\PRN231Fall2024_SE1714_Group5_ARS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341420CC-6F34-46BA-942E-B696453FB151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B105B497-03EA-4D69-9038-F406E3773264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>FlightNumber</t>
   </si>
@@ -436,7 +436,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,10 +511,62 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C3" s="2"/>
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45635.375</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>1490000</v>
+      </c>
+      <c r="H3">
+        <v>2000000</v>
+      </c>
+      <c r="I3">
+        <v>50000000</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C4" s="2"/>
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45635.375</v>
+      </c>
+      <c r="D4">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>1490000</v>
+      </c>
+      <c r="H4">
+        <v>2000000</v>
+      </c>
+      <c r="I4">
+        <v>50000000</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>

</xml_diff>